<commit_message>
update data extraction files and processed dataset
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Altuna-Etxabe.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Altuna-Etxabe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623866E1-E4D6-4478-88D4-9ADB3600891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDC67EF-9744-45C0-A1EE-683EF742FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2326,7 +2326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6343" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6343" uniqueCount="654">
   <si>
     <t>SearchID</t>
   </si>
@@ -4111,9 +4111,6 @@
   </si>
   <si>
     <t>Revenue</t>
-  </si>
-  <si>
-    <t>Biolobical parameters (e.g. growth parameters, recruitment)</t>
   </si>
   <si>
     <t>The positive effects expected from protecting hake nursery grounds are only marginally related to a reduction in hake recruits fishing mortality</t>
@@ -4283,6 +4280,15 @@
   </si>
   <si>
     <t>Sparus aurata _ Thunnus thynnus _ Scomber scombrus _ Coryphaena hippurus _ Dicentrarchus labrax _ Euthynnus alletteratus _ Trachurus trachurus _ Lichia amia _ Pomatomus saltatrix _ Lithognathus mormyrus _ Anguilla anguilla _ Boops boops _ Diplodus sargus sargus _ Sarda sarda _ Pagellus erythrinus _ Merluccius merluccius _ Scomber colias _ Mugil spp. _ Merlangius merlangus _ Spicara maena _ Chelidonichthys lucerna _ Oblada melanura _ Platichthys flesus _ Ombrina cirrosa _ Scophthalmus rhombus _ Scophthalmus maximus</t>
+  </si>
+  <si>
+    <t>Bycatch mortality</t>
+  </si>
+  <si>
+    <t>Trawling impact (change in mean annual trawling frequency as compared to the baseline scenario)</t>
+  </si>
+  <si>
+    <t>Biological parameters (e.g. growth parameters, recruitment)</t>
   </si>
 </sst>
 </file>
@@ -4797,7 +4803,7 @@
   <dimension ref="A1:AX151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT156" sqref="AT156"/>
+      <selection activeCell="AU5" sqref="AU5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5707,7 +5713,7 @@
         <v>459</v>
       </c>
       <c r="AU7" s="14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AV7" s="14" t="s">
         <v>201</v>
@@ -5841,10 +5847,10 @@
         <v>459</v>
       </c>
       <c r="AU8" s="19" t="s">
-        <v>619</v>
+        <v>651</v>
       </c>
       <c r="AV8" s="10" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="AW8" s="10" t="s">
         <v>211</v>
@@ -5972,10 +5978,10 @@
         <v>459</v>
       </c>
       <c r="AU9" s="19" t="s">
-        <v>619</v>
+        <v>651</v>
       </c>
       <c r="AV9" s="10" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="AW9" s="10" t="s">
         <v>211</v>
@@ -6106,10 +6112,10 @@
         <v>459</v>
       </c>
       <c r="AU10" s="21" t="s">
-        <v>619</v>
+        <v>652</v>
       </c>
       <c r="AV10" s="10" t="s">
-        <v>201</v>
+        <v>115</v>
       </c>
       <c r="AW10" s="10" t="s">
         <v>211</v>
@@ -6228,7 +6234,7 @@
         <v>464</v>
       </c>
       <c r="AP11" s="14" t="s">
-        <v>595</v>
+        <v>653</v>
       </c>
       <c r="AQ11" s="14" t="s">
         <v>166</v>
@@ -6249,7 +6255,7 @@
         <v>209</v>
       </c>
       <c r="AX11" s="14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="12" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -6362,7 +6368,7 @@
         <v>464</v>
       </c>
       <c r="AP12" s="10" t="s">
-        <v>595</v>
+        <v>653</v>
       </c>
       <c r="AQ12" s="10" t="s">
         <v>166</v>
@@ -6383,7 +6389,7 @@
         <v>209</v>
       </c>
       <c r="AX12" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -6496,7 +6502,7 @@
         <v>464</v>
       </c>
       <c r="AP13" s="10" t="s">
-        <v>595</v>
+        <v>653</v>
       </c>
       <c r="AQ13" s="10" t="s">
         <v>166</v>
@@ -6520,7 +6526,7 @@
         <v>209</v>
       </c>
       <c r="AX13" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -6633,7 +6639,7 @@
         <v>464</v>
       </c>
       <c r="AP14" s="10" t="s">
-        <v>595</v>
+        <v>653</v>
       </c>
       <c r="AQ14" s="10" t="s">
         <v>166</v>
@@ -6657,7 +6663,7 @@
         <v>209</v>
       </c>
       <c r="AX14" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -7267,7 +7273,7 @@
         <v>209</v>
       </c>
       <c r="AX19" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -7389,7 +7395,7 @@
         <v>209</v>
       </c>
       <c r="AX20" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="21" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -7496,13 +7502,13 @@
         <v>526</v>
       </c>
       <c r="AP21" s="14" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AQ21" s="14" t="s">
         <v>152</v>
       </c>
       <c r="AU21" s="14" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AV21" s="14" t="s">
         <v>201</v>
@@ -7618,13 +7624,13 @@
         <v>526</v>
       </c>
       <c r="AP22" s="19" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AQ22" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU22" s="19" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AV22" s="10" t="s">
         <v>201</v>
@@ -7743,13 +7749,13 @@
         <v>526</v>
       </c>
       <c r="AP23" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AQ23" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU23" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AV23" s="10" t="s">
         <v>201</v>
@@ -7868,7 +7874,7 @@
         <v>521</v>
       </c>
       <c r="AP24" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AQ24" s="10" t="s">
         <v>166</v>
@@ -7877,7 +7883,7 @@
         <v>241</v>
       </c>
       <c r="AU24" s="18" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AV24" s="12" t="s">
         <v>214</v>
@@ -7886,7 +7892,7 @@
         <v>211</v>
       </c>
       <c r="AX24" s="12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="25" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -9142,7 +9148,7 @@
         <v>313</v>
       </c>
       <c r="Z34" s="14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA34" s="14">
         <v>3</v>
@@ -9193,7 +9199,7 @@
         <v>495</v>
       </c>
       <c r="AU34" s="15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV34" s="14" t="s">
         <v>201</v>
@@ -9202,7 +9208,7 @@
         <v>210</v>
       </c>
       <c r="AX34" s="23" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="35" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9279,7 +9285,7 @@
         <v>313</v>
       </c>
       <c r="Z35" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA35" s="19">
         <v>3</v>
@@ -9327,7 +9333,7 @@
         <v>496</v>
       </c>
       <c r="AU35" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV35" s="19" t="s">
         <v>201</v>
@@ -9336,7 +9342,7 @@
         <v>210</v>
       </c>
       <c r="AX35" s="24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="36" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9413,7 +9419,7 @@
         <v>313</v>
       </c>
       <c r="Z36" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA36" s="19">
         <v>3</v>
@@ -9461,7 +9467,7 @@
         <v>497</v>
       </c>
       <c r="AU36" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV36" s="19" t="s">
         <v>201</v>
@@ -9470,7 +9476,7 @@
         <v>210</v>
       </c>
       <c r="AX36" s="24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="37" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9547,7 +9553,7 @@
         <v>313</v>
       </c>
       <c r="Z37" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA37" s="19">
         <v>3</v>
@@ -9595,7 +9601,7 @@
         <v>495</v>
       </c>
       <c r="AU37" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV37" s="19" t="s">
         <v>201</v>
@@ -9604,7 +9610,7 @@
         <v>210</v>
       </c>
       <c r="AX37" s="24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="38" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9681,7 +9687,7 @@
         <v>313</v>
       </c>
       <c r="Z38" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA38" s="19">
         <v>3</v>
@@ -9726,7 +9732,7 @@
         <v>496</v>
       </c>
       <c r="AU38" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV38" s="19" t="s">
         <v>201</v>
@@ -9735,7 +9741,7 @@
         <v>210</v>
       </c>
       <c r="AX38" s="24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="39" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9812,7 +9818,7 @@
         <v>313</v>
       </c>
       <c r="Z39" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA39" s="19">
         <v>3</v>
@@ -9857,7 +9863,7 @@
         <v>497</v>
       </c>
       <c r="AU39" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV39" s="19" t="s">
         <v>201</v>
@@ -9866,7 +9872,7 @@
         <v>210</v>
       </c>
       <c r="AX39" s="24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -9943,7 +9949,7 @@
         <v>313</v>
       </c>
       <c r="Z40" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA40" s="19">
         <v>3</v>
@@ -9970,7 +9976,7 @@
         <v>152</v>
       </c>
       <c r="AL40" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AM40" s="19" t="s">
         <v>234</v>
@@ -9997,7 +10003,7 @@
         <v>495</v>
       </c>
       <c r="AU40" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV40" s="19" t="s">
         <v>201</v>
@@ -10006,7 +10012,7 @@
         <v>212</v>
       </c>
       <c r="AX40" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10083,7 +10089,7 @@
         <v>313</v>
       </c>
       <c r="Z41" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA41" s="19">
         <v>3</v>
@@ -10110,7 +10116,7 @@
         <v>152</v>
       </c>
       <c r="AL41" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AM41" s="19" t="s">
         <v>234</v>
@@ -10134,7 +10140,7 @@
         <v>496</v>
       </c>
       <c r="AU41" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV41" s="19" t="s">
         <v>201</v>
@@ -10143,7 +10149,7 @@
         <v>212</v>
       </c>
       <c r="AX41" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10220,7 +10226,7 @@
         <v>313</v>
       </c>
       <c r="Z42" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA42" s="19">
         <v>3</v>
@@ -10247,7 +10253,7 @@
         <v>152</v>
       </c>
       <c r="AL42" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AM42" s="19" t="s">
         <v>234</v>
@@ -10271,7 +10277,7 @@
         <v>497</v>
       </c>
       <c r="AU42" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV42" s="19" t="s">
         <v>201</v>
@@ -10280,7 +10286,7 @@
         <v>212</v>
       </c>
       <c r="AX42" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="43" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10357,7 +10363,7 @@
         <v>313</v>
       </c>
       <c r="Z43" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA43" s="19">
         <v>3</v>
@@ -10384,7 +10390,7 @@
         <v>152</v>
       </c>
       <c r="AL43" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AM43" s="19" t="s">
         <v>235</v>
@@ -10408,7 +10414,7 @@
         <v>495</v>
       </c>
       <c r="AU43" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV43" s="19" t="s">
         <v>201</v>
@@ -10417,7 +10423,7 @@
         <v>209</v>
       </c>
       <c r="AX43" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="44" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10494,7 +10500,7 @@
         <v>313</v>
       </c>
       <c r="Z44" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA44" s="19">
         <v>3</v>
@@ -10521,7 +10527,7 @@
         <v>152</v>
       </c>
       <c r="AL44" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AM44" s="19" t="s">
         <v>235</v>
@@ -10542,7 +10548,7 @@
         <v>496</v>
       </c>
       <c r="AU44" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV44" s="19" t="s">
         <v>201</v>
@@ -10551,7 +10557,7 @@
         <v>209</v>
       </c>
       <c r="AX44" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="45" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10628,7 +10634,7 @@
         <v>313</v>
       </c>
       <c r="Z45" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA45" s="19">
         <v>3</v>
@@ -10655,7 +10661,7 @@
         <v>152</v>
       </c>
       <c r="AL45" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AM45" s="19" t="s">
         <v>235</v>
@@ -10676,7 +10682,7 @@
         <v>497</v>
       </c>
       <c r="AU45" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AV45" s="19" t="s">
         <v>201</v>
@@ -10685,7 +10691,7 @@
         <v>209</v>
       </c>
       <c r="AX45" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="46" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10762,7 +10768,7 @@
         <v>313</v>
       </c>
       <c r="Z46" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA46" s="19">
         <v>3</v>
@@ -10811,7 +10817,7 @@
         <v>497</v>
       </c>
       <c r="AU46" s="20" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AV46" s="19" t="s">
         <v>204</v>
@@ -10820,7 +10826,7 @@
         <v>212</v>
       </c>
       <c r="AX46" s="24" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="47" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -10897,7 +10903,7 @@
         <v>313</v>
       </c>
       <c r="Z47" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA47" s="19">
         <v>3</v>
@@ -10948,7 +10954,7 @@
         <v>495</v>
       </c>
       <c r="AU47" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV47" s="19" t="s">
         <v>207</v>
@@ -10957,7 +10963,7 @@
         <v>209</v>
       </c>
       <c r="AX47" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -11034,7 +11040,7 @@
         <v>313</v>
       </c>
       <c r="Z48" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA48" s="19">
         <v>3</v>
@@ -11082,7 +11088,7 @@
         <v>496</v>
       </c>
       <c r="AU48" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV48" s="19" t="s">
         <v>207</v>
@@ -11091,7 +11097,7 @@
         <v>209</v>
       </c>
       <c r="AX48" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -11168,7 +11174,7 @@
         <v>313</v>
       </c>
       <c r="Z49" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA49" s="19">
         <v>3</v>
@@ -11216,7 +11222,7 @@
         <v>497</v>
       </c>
       <c r="AU49" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV49" s="19" t="s">
         <v>207</v>
@@ -11225,7 +11231,7 @@
         <v>209</v>
       </c>
       <c r="AX49" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="50" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -11302,7 +11308,7 @@
         <v>313</v>
       </c>
       <c r="Z50" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA50" s="19">
         <v>3</v>
@@ -11350,7 +11356,7 @@
         <v>495</v>
       </c>
       <c r="AU50" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV50" s="19" t="s">
         <v>207</v>
@@ -11359,7 +11365,7 @@
         <v>209</v>
       </c>
       <c r="AX50" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="51" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -11436,7 +11442,7 @@
         <v>313</v>
       </c>
       <c r="Z51" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA51" s="19">
         <v>3</v>
@@ -11481,7 +11487,7 @@
         <v>496</v>
       </c>
       <c r="AU51" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV51" s="19" t="s">
         <v>207</v>
@@ -11490,7 +11496,7 @@
         <v>209</v>
       </c>
       <c r="AX51" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="52" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -11567,7 +11573,7 @@
         <v>313</v>
       </c>
       <c r="Z52" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA52" s="19">
         <v>3</v>
@@ -11612,7 +11618,7 @@
         <v>497</v>
       </c>
       <c r="AU52" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AV52" s="19" t="s">
         <v>207</v>
@@ -11621,7 +11627,7 @@
         <v>209</v>
       </c>
       <c r="AX52" s="24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="53" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -11725,10 +11731,10 @@
         <v>164</v>
       </c>
       <c r="AO53" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP53" s="14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ53" s="14" t="s">
         <v>166</v>
@@ -11743,7 +11749,7 @@
         <v>502</v>
       </c>
       <c r="AU53" s="14" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV53" s="14" t="s">
         <v>201</v>
@@ -11752,7 +11758,7 @@
         <v>210</v>
       </c>
       <c r="AX53" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="54" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -11856,10 +11862,10 @@
         <v>164</v>
       </c>
       <c r="AO54" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP54" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ54" s="10" t="s">
         <v>166</v>
@@ -11874,7 +11880,7 @@
         <v>503</v>
       </c>
       <c r="AU54" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV54" s="10" t="s">
         <v>201</v>
@@ -11883,7 +11889,7 @@
         <v>210</v>
       </c>
       <c r="AX54" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="55" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -11987,10 +11993,10 @@
         <v>164</v>
       </c>
       <c r="AO55" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP55" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ55" s="10" t="s">
         <v>166</v>
@@ -12005,7 +12011,7 @@
         <v>504</v>
       </c>
       <c r="AU55" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV55" s="10" t="s">
         <v>201</v>
@@ -12014,7 +12020,7 @@
         <v>210</v>
       </c>
       <c r="AX55" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="56" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12118,10 +12124,10 @@
         <v>164</v>
       </c>
       <c r="AO56" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP56" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ56" s="10" t="s">
         <v>166</v>
@@ -12136,7 +12142,7 @@
         <v>505</v>
       </c>
       <c r="AU56" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV56" s="10" t="s">
         <v>201</v>
@@ -12145,7 +12151,7 @@
         <v>210</v>
       </c>
       <c r="AX56" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12249,10 +12255,10 @@
         <v>164</v>
       </c>
       <c r="AO57" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP57" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ57" s="10" t="s">
         <v>166</v>
@@ -12267,7 +12273,7 @@
         <v>501</v>
       </c>
       <c r="AU57" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV57" s="10" t="s">
         <v>201</v>
@@ -12276,7 +12282,7 @@
         <v>210</v>
       </c>
       <c r="AX57" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="58" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12380,10 +12386,10 @@
         <v>164</v>
       </c>
       <c r="AO58" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP58" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ58" s="10" t="s">
         <v>166</v>
@@ -12398,7 +12404,7 @@
         <v>502</v>
       </c>
       <c r="AU58" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV58" s="10" t="s">
         <v>201</v>
@@ -12407,7 +12413,7 @@
         <v>210</v>
       </c>
       <c r="AX58" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="59" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12511,10 +12517,10 @@
         <v>164</v>
       </c>
       <c r="AO59" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP59" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ59" s="10" t="s">
         <v>166</v>
@@ -12529,7 +12535,7 @@
         <v>503</v>
       </c>
       <c r="AU59" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV59" s="10" t="s">
         <v>201</v>
@@ -12538,7 +12544,7 @@
         <v>210</v>
       </c>
       <c r="AX59" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="60" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12642,10 +12648,10 @@
         <v>164</v>
       </c>
       <c r="AO60" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP60" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ60" s="10" t="s">
         <v>166</v>
@@ -12660,7 +12666,7 @@
         <v>504</v>
       </c>
       <c r="AU60" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV60" s="10" t="s">
         <v>201</v>
@@ -12669,7 +12675,7 @@
         <v>210</v>
       </c>
       <c r="AX60" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="61" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12773,10 +12779,10 @@
         <v>164</v>
       </c>
       <c r="AO61" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP61" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ61" s="10" t="s">
         <v>166</v>
@@ -12791,7 +12797,7 @@
         <v>505</v>
       </c>
       <c r="AU61" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV61" s="10" t="s">
         <v>201</v>
@@ -12800,7 +12806,7 @@
         <v>210</v>
       </c>
       <c r="AX61" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="62" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -12904,10 +12910,10 @@
         <v>164</v>
       </c>
       <c r="AO62" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP62" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ62" s="10" t="s">
         <v>166</v>
@@ -12922,7 +12928,7 @@
         <v>501</v>
       </c>
       <c r="AU62" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV62" s="10" t="s">
         <v>201</v>
@@ -12931,7 +12937,7 @@
         <v>210</v>
       </c>
       <c r="AX62" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="63" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13038,10 +13044,10 @@
         <v>164</v>
       </c>
       <c r="AO63" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP63" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ63" s="10" t="s">
         <v>166</v>
@@ -13056,7 +13062,7 @@
         <v>502</v>
       </c>
       <c r="AU63" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV63" s="10" t="s">
         <v>201</v>
@@ -13065,7 +13071,7 @@
         <v>210</v>
       </c>
       <c r="AX63" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="64" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13172,10 +13178,10 @@
         <v>164</v>
       </c>
       <c r="AO64" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP64" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ64" s="10" t="s">
         <v>166</v>
@@ -13190,7 +13196,7 @@
         <v>503</v>
       </c>
       <c r="AU64" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV64" s="10" t="s">
         <v>201</v>
@@ -13199,7 +13205,7 @@
         <v>210</v>
       </c>
       <c r="AX64" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="65" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13306,10 +13312,10 @@
         <v>164</v>
       </c>
       <c r="AO65" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP65" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ65" s="10" t="s">
         <v>166</v>
@@ -13324,7 +13330,7 @@
         <v>504</v>
       </c>
       <c r="AU65" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV65" s="10" t="s">
         <v>201</v>
@@ -13333,7 +13339,7 @@
         <v>210</v>
       </c>
       <c r="AX65" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="66" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13440,10 +13446,10 @@
         <v>164</v>
       </c>
       <c r="AO66" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP66" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ66" s="10" t="s">
         <v>166</v>
@@ -13458,7 +13464,7 @@
         <v>505</v>
       </c>
       <c r="AU66" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV66" s="10" t="s">
         <v>201</v>
@@ -13467,7 +13473,7 @@
         <v>210</v>
       </c>
       <c r="AX66" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13574,10 +13580,10 @@
         <v>164</v>
       </c>
       <c r="AO67" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AP67" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AQ67" s="10" t="s">
         <v>166</v>
@@ -13592,7 +13598,7 @@
         <v>501</v>
       </c>
       <c r="AU67" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AV67" s="10" t="s">
         <v>201</v>
@@ -13601,7 +13607,7 @@
         <v>210</v>
       </c>
       <c r="AX67" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="68" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -13675,7 +13681,7 @@
         <v>69</v>
       </c>
       <c r="Z68" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AA68" s="14">
         <v>2</v>
@@ -13717,7 +13723,7 @@
         <v>509</v>
       </c>
       <c r="AU68" s="14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AV68" s="14" t="s">
         <v>201</v>
@@ -13726,7 +13732,7 @@
         <v>209</v>
       </c>
       <c r="AX68" s="15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="69" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -13800,7 +13806,7 @@
         <v>69</v>
       </c>
       <c r="Z69" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AA69" s="10">
         <v>2</v>
@@ -13842,7 +13848,7 @@
         <v>509</v>
       </c>
       <c r="AU69" s="14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AV69" s="10" t="s">
         <v>201</v>
@@ -13851,7 +13857,7 @@
         <v>209</v>
       </c>
       <c r="AX69" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="70" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -13925,7 +13931,7 @@
         <v>217</v>
       </c>
       <c r="Z70" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AA70" s="14">
         <v>3</v>
@@ -14053,7 +14059,7 @@
         <v>217</v>
       </c>
       <c r="Z71" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AA71" s="10">
         <v>3</v>
@@ -14178,7 +14184,7 @@
         <v>217</v>
       </c>
       <c r="Z72" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AA72" s="10">
         <v>3</v>
@@ -14312,7 +14318,7 @@
         <v>217</v>
       </c>
       <c r="Z73" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AA73" s="10">
         <v>3</v>
@@ -14446,7 +14452,7 @@
         <v>217</v>
       </c>
       <c r="Z74" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AA74" s="10">
         <v>3</v>
@@ -14610,7 +14616,7 @@
         <v>164</v>
       </c>
       <c r="AO75" s="14" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ75" s="14" t="s">
         <v>166</v>
@@ -14741,7 +14747,7 @@
         <v>162</v>
       </c>
       <c r="AO76" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ76" s="10" t="s">
         <v>166</v>
@@ -14872,7 +14878,7 @@
         <v>162</v>
       </c>
       <c r="AO77" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ77" s="10" t="s">
         <v>166</v>
@@ -15000,7 +15006,7 @@
         <v>164</v>
       </c>
       <c r="AO78" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ78" s="10" t="s">
         <v>166</v>
@@ -15128,7 +15134,7 @@
         <v>162</v>
       </c>
       <c r="AO79" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ79" s="10" t="s">
         <v>166</v>
@@ -15256,7 +15262,7 @@
         <v>162</v>
       </c>
       <c r="AO80" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ80" s="10" t="s">
         <v>166</v>
@@ -15381,7 +15387,7 @@
         <v>164</v>
       </c>
       <c r="AO81" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ81" s="10" t="s">
         <v>166</v>
@@ -15509,7 +15515,7 @@
         <v>162</v>
       </c>
       <c r="AO82" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ82" s="10" t="s">
         <v>166</v>
@@ -15637,7 +15643,7 @@
         <v>162</v>
       </c>
       <c r="AO83" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ83" s="10" t="s">
         <v>166</v>
@@ -15762,7 +15768,7 @@
         <v>164</v>
       </c>
       <c r="AO84" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ84" s="10" t="s">
         <v>166</v>
@@ -15893,7 +15899,7 @@
         <v>162</v>
       </c>
       <c r="AO85" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ85" s="10" t="s">
         <v>166</v>
@@ -16024,7 +16030,7 @@
         <v>162</v>
       </c>
       <c r="AO86" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ86" s="10" t="s">
         <v>166</v>
@@ -16152,7 +16158,7 @@
         <v>164</v>
       </c>
       <c r="AO87" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ87" s="10" t="s">
         <v>166</v>
@@ -16280,7 +16286,7 @@
         <v>162</v>
       </c>
       <c r="AO88" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ88" s="10" t="s">
         <v>166</v>
@@ -16408,7 +16414,7 @@
         <v>162</v>
       </c>
       <c r="AO89" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ89" s="10" t="s">
         <v>166</v>
@@ -16533,7 +16539,7 @@
         <v>164</v>
       </c>
       <c r="AO90" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ90" s="10" t="s">
         <v>166</v>
@@ -16661,7 +16667,7 @@
         <v>162</v>
       </c>
       <c r="AO91" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ91" s="10" t="s">
         <v>166</v>
@@ -16789,7 +16795,7 @@
         <v>162</v>
       </c>
       <c r="AO92" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ92" s="10" t="s">
         <v>166</v>
@@ -16914,7 +16920,7 @@
         <v>162</v>
       </c>
       <c r="AO93" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ93" s="10" t="s">
         <v>166</v>
@@ -17045,7 +17051,7 @@
         <v>162</v>
       </c>
       <c r="AO94" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ94" s="10" t="s">
         <v>166</v>
@@ -17176,7 +17182,7 @@
         <v>162</v>
       </c>
       <c r="AO95" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ95" s="10" t="s">
         <v>166</v>
@@ -17304,7 +17310,7 @@
         <v>162</v>
       </c>
       <c r="AO96" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ96" s="10" t="s">
         <v>166</v>
@@ -17432,7 +17438,7 @@
         <v>162</v>
       </c>
       <c r="AO97" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ97" s="10" t="s">
         <v>166</v>
@@ -17560,7 +17566,7 @@
         <v>162</v>
       </c>
       <c r="AO98" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ98" s="10" t="s">
         <v>166</v>
@@ -17685,7 +17691,7 @@
         <v>162</v>
       </c>
       <c r="AO99" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ99" s="10" t="s">
         <v>166</v>
@@ -17816,7 +17822,7 @@
         <v>162</v>
       </c>
       <c r="AO100" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ100" s="10" t="s">
         <v>166</v>
@@ -17947,7 +17953,7 @@
         <v>162</v>
       </c>
       <c r="AO101" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ101" s="10" t="s">
         <v>166</v>
@@ -18075,7 +18081,7 @@
         <v>162</v>
       </c>
       <c r="AO102" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ102" s="10" t="s">
         <v>166</v>
@@ -18203,7 +18209,7 @@
         <v>162</v>
       </c>
       <c r="AO103" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ103" s="10" t="s">
         <v>166</v>
@@ -18331,7 +18337,7 @@
         <v>162</v>
       </c>
       <c r="AO104" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ104" s="10" t="s">
         <v>166</v>
@@ -18456,7 +18462,7 @@
         <v>162</v>
       </c>
       <c r="AO105" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ105" s="10" t="s">
         <v>166</v>
@@ -18587,7 +18593,7 @@
         <v>162</v>
       </c>
       <c r="AO106" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ106" s="10" t="s">
         <v>166</v>
@@ -18718,7 +18724,7 @@
         <v>162</v>
       </c>
       <c r="AO107" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ107" s="10" t="s">
         <v>166</v>
@@ -18846,7 +18852,7 @@
         <v>162</v>
       </c>
       <c r="AO108" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ108" s="10" t="s">
         <v>166</v>
@@ -18974,7 +18980,7 @@
         <v>162</v>
       </c>
       <c r="AO109" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ109" s="10" t="s">
         <v>166</v>
@@ -19102,7 +19108,7 @@
         <v>162</v>
       </c>
       <c r="AO110" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ110" s="10" t="s">
         <v>166</v>
@@ -19230,7 +19236,7 @@
         <v>162</v>
       </c>
       <c r="AO111" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ111" s="14" t="s">
         <v>167</v>
@@ -19245,7 +19251,7 @@
         <v>480</v>
       </c>
       <c r="AU111" s="14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV111" s="14" t="s">
         <v>206</v>
@@ -19352,7 +19358,7 @@
         <v>119</v>
       </c>
       <c r="AL112" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AM112" s="10" t="s">
         <v>234</v>
@@ -19361,7 +19367,7 @@
         <v>162</v>
       </c>
       <c r="AO112" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ112" s="10" t="s">
         <v>167</v>
@@ -19376,7 +19382,7 @@
         <v>480</v>
       </c>
       <c r="AU112" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV112" s="10" t="s">
         <v>206</v>
@@ -19495,7 +19501,7 @@
         <v>162</v>
       </c>
       <c r="AO113" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ113" s="10" t="s">
         <v>167</v>
@@ -19510,7 +19516,7 @@
         <v>480</v>
       </c>
       <c r="AU113" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV113" s="10" t="s">
         <v>206</v>
@@ -19629,7 +19635,7 @@
         <v>162</v>
       </c>
       <c r="AO114" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ114" s="10" t="s">
         <v>167</v>
@@ -19644,7 +19650,7 @@
         <v>480</v>
       </c>
       <c r="AU114" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV114" s="10" t="s">
         <v>206</v>
@@ -19757,7 +19763,7 @@
         <v>162</v>
       </c>
       <c r="AO115" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ115" s="10" t="s">
         <v>167</v>
@@ -19772,7 +19778,7 @@
         <v>480</v>
       </c>
       <c r="AU115" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV115" s="10" t="s">
         <v>206</v>
@@ -19876,7 +19882,7 @@
         <v>119</v>
       </c>
       <c r="AL116" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AM116" s="10" t="s">
         <v>234</v>
@@ -19885,7 +19891,7 @@
         <v>162</v>
       </c>
       <c r="AO116" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ116" s="10" t="s">
         <v>167</v>
@@ -19900,7 +19906,7 @@
         <v>480</v>
       </c>
       <c r="AU116" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV116" s="10" t="s">
         <v>206</v>
@@ -20016,7 +20022,7 @@
         <v>162</v>
       </c>
       <c r="AO117" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ117" s="10" t="s">
         <v>167</v>
@@ -20031,7 +20037,7 @@
         <v>480</v>
       </c>
       <c r="AU117" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV117" s="10" t="s">
         <v>206</v>
@@ -20147,7 +20153,7 @@
         <v>162</v>
       </c>
       <c r="AO118" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AQ118" s="10" t="s">
         <v>167</v>
@@ -20162,7 +20168,7 @@
         <v>480</v>
       </c>
       <c r="AU118" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AV118" s="10" t="s">
         <v>206</v>
@@ -20245,7 +20251,7 @@
         <v>71</v>
       </c>
       <c r="Z119" s="14" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AA119" s="14">
         <v>3</v>
@@ -20272,10 +20278,10 @@
         <v>161</v>
       </c>
       <c r="AO119" s="16" t="s">
+        <v>616</v>
+      </c>
+      <c r="AP119" s="14" t="s">
         <v>617</v>
-      </c>
-      <c r="AP119" s="14" t="s">
-        <v>618</v>
       </c>
       <c r="AQ119" s="14" t="s">
         <v>166</v>
@@ -20296,7 +20302,7 @@
         <v>209</v>
       </c>
       <c r="AX119" s="14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="120" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -20397,10 +20403,10 @@
         <v>161</v>
       </c>
       <c r="AO120" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="AP120" s="10" t="s">
         <v>617</v>
-      </c>
-      <c r="AP120" s="10" t="s">
-        <v>618</v>
       </c>
       <c r="AQ120" s="10" t="s">
         <v>166</v>
@@ -20421,7 +20427,7 @@
         <v>209</v>
       </c>
       <c r="AX120" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="121" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -20522,10 +20528,10 @@
         <v>161</v>
       </c>
       <c r="AO121" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="AP121" s="10" t="s">
         <v>617</v>
-      </c>
-      <c r="AP121" s="10" t="s">
-        <v>618</v>
       </c>
       <c r="AQ121" s="10" t="s">
         <v>166</v>
@@ -20546,7 +20552,7 @@
         <v>209</v>
       </c>
       <c r="AX121" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="122" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -20647,10 +20653,10 @@
         <v>161</v>
       </c>
       <c r="AO122" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="AP122" s="10" t="s">
         <v>617</v>
-      </c>
-      <c r="AP122" s="10" t="s">
-        <v>618</v>
       </c>
       <c r="AQ122" s="10" t="s">
         <v>166</v>
@@ -20671,7 +20677,7 @@
         <v>209</v>
       </c>
       <c r="AX122" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="123" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -21010,7 +21016,7 @@
         <v>313</v>
       </c>
       <c r="Z125" s="14" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA125" s="14">
         <v>3</v>
@@ -21064,7 +21070,7 @@
         <v>212</v>
       </c>
       <c r="AX125" s="14" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="126" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -21141,7 +21147,7 @@
         <v>313</v>
       </c>
       <c r="Z126" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA126" s="19">
         <v>3</v>
@@ -21198,7 +21204,7 @@
         <v>210</v>
       </c>
       <c r="AX126" s="19" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="127" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -21275,7 +21281,7 @@
         <v>313</v>
       </c>
       <c r="Z127" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA127" s="19">
         <v>3</v>
@@ -21329,7 +21335,7 @@
         <v>212</v>
       </c>
       <c r="AX127" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="128" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -21406,7 +21412,7 @@
         <v>313</v>
       </c>
       <c r="Z128" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA128" s="19">
         <v>3</v>
@@ -21543,7 +21549,7 @@
         <v>313</v>
       </c>
       <c r="Z129" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA129" s="19">
         <v>3</v>
@@ -21600,7 +21606,7 @@
         <v>212</v>
       </c>
       <c r="AX129" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="130" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -21677,7 +21683,7 @@
         <v>313</v>
       </c>
       <c r="Z130" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA130" s="19">
         <v>3</v>
@@ -21811,7 +21817,7 @@
         <v>313</v>
       </c>
       <c r="Z131" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA131" s="19">
         <v>3</v>
@@ -21862,7 +21868,7 @@
         <v>212</v>
       </c>
       <c r="AX131" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="132" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -21939,7 +21945,7 @@
         <v>313</v>
       </c>
       <c r="Z132" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA132" s="19">
         <v>3</v>
@@ -22076,7 +22082,7 @@
         <v>313</v>
       </c>
       <c r="Z133" s="21" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AA133" s="21">
         <v>3</v>
@@ -22237,7 +22243,7 @@
         <v>161</v>
       </c>
       <c r="AO134" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AP134" s="14" t="s">
         <v>522</v>
@@ -22250,7 +22256,7 @@
       </c>
       <c r="AT134" s="16"/>
       <c r="AU134" s="16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AV134" s="16" t="s">
         <v>214</v>
@@ -22259,7 +22265,7 @@
         <v>211</v>
       </c>
       <c r="AX134" s="16" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="135" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -22366,7 +22372,7 @@
         <v>161</v>
       </c>
       <c r="AO135" s="27" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AP135" s="21" t="s">
         <v>522</v>
@@ -22379,7 +22385,7 @@
       </c>
       <c r="AT135" s="27"/>
       <c r="AU135" s="27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AV135" s="27" t="s">
         <v>214</v>
@@ -22388,7 +22394,7 @@
         <v>211</v>
       </c>
       <c r="AX135" s="27" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="136" spans="1:50" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -22507,7 +22513,7 @@
         <v>538</v>
       </c>
       <c r="AU136" s="14" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AV136" s="14" t="s">
         <v>201</v>
@@ -22635,7 +22641,7 @@
         <v>538</v>
       </c>
       <c r="AU137" s="19" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AV137" s="19" t="s">
         <v>201</v>
@@ -22763,7 +22769,7 @@
         <v>538</v>
       </c>
       <c r="AU138" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AV138" s="21" t="s">
         <v>201</v>
@@ -22879,7 +22885,7 @@
         <v>162</v>
       </c>
       <c r="AO139" s="19" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AP139" s="13" t="s">
         <v>537</v>
@@ -22906,7 +22912,7 @@
         <v>210</v>
       </c>
       <c r="AX139" s="13" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="140" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23010,7 +23016,7 @@
         <v>162</v>
       </c>
       <c r="AO140" s="19" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AP140" s="13" t="s">
         <v>537</v>
@@ -23037,7 +23043,7 @@
         <v>210</v>
       </c>
       <c r="AX140" s="13" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="141" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -23151,7 +23157,7 @@
         <v>162</v>
       </c>
       <c r="AO141" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AP141" s="22" t="s">
         <v>537</v>
@@ -23178,7 +23184,7 @@
         <v>210</v>
       </c>
       <c r="AX141" s="13" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="142" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23280,22 +23286,22 @@
         <v>132</v>
       </c>
       <c r="AL142" s="14" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AM142" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO142" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP142" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ142" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU142" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV142" s="10" t="s">
         <v>201</v>
@@ -23304,7 +23310,7 @@
         <v>209</v>
       </c>
       <c r="AX142" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="143" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23406,22 +23412,22 @@
         <v>146</v>
       </c>
       <c r="AL143" s="19" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AM143" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO143" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP143" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ143" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU143" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV143" s="10" t="s">
         <v>201</v>
@@ -23430,7 +23436,7 @@
         <v>209</v>
       </c>
       <c r="AX143" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="144" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23532,22 +23538,22 @@
         <v>149</v>
       </c>
       <c r="AL144" s="19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AM144" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO144" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP144" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ144" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU144" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV144" s="10" t="s">
         <v>201</v>
@@ -23556,7 +23562,7 @@
         <v>209</v>
       </c>
       <c r="AX144" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="145" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23658,22 +23664,22 @@
         <v>133</v>
       </c>
       <c r="AL145" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AM145" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO145" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP145" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ145" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU145" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV145" s="10" t="s">
         <v>201</v>
@@ -23682,7 +23688,7 @@
         <v>209</v>
       </c>
       <c r="AX145" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="146" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23784,22 +23790,22 @@
         <v>147</v>
       </c>
       <c r="AL146" s="19" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AM146" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO146" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP146" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ146" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU146" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV146" s="10" t="s">
         <v>201</v>
@@ -23808,7 +23814,7 @@
         <v>209</v>
       </c>
       <c r="AX146" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="147" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23907,22 +23913,22 @@
         <v>132</v>
       </c>
       <c r="AL147" s="19" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AM147" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO147" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP147" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ147" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU147" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV147" s="10" t="s">
         <v>201</v>
@@ -23931,7 +23937,7 @@
         <v>209</v>
       </c>
       <c r="AX147" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="148" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -23997,7 +24003,7 @@
         <v>59</v>
       </c>
       <c r="V148" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W148" s="10" t="s">
         <v>53</v>
@@ -24030,22 +24036,22 @@
         <v>146</v>
       </c>
       <c r="AL148" s="19" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AM148" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO148" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP148" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ148" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU148" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV148" s="10" t="s">
         <v>201</v>
@@ -24054,7 +24060,7 @@
         <v>209</v>
       </c>
       <c r="AX148" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="149" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -24153,22 +24159,22 @@
         <v>149</v>
       </c>
       <c r="AL149" s="19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AM149" s="10" t="s">
         <v>234</v>
       </c>
       <c r="AO149" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP149" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ149" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU149" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV149" s="10" t="s">
         <v>201</v>
@@ -24177,7 +24183,7 @@
         <v>209</v>
       </c>
       <c r="AX149" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="150" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -24243,7 +24249,7 @@
         <v>59</v>
       </c>
       <c r="V150" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W150" s="10" t="s">
         <v>53</v>
@@ -24278,22 +24284,22 @@
       <c r="AJ150" s="19"/>
       <c r="AK150" s="19"/>
       <c r="AL150" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AM150" s="19" t="s">
         <v>234</v>
       </c>
       <c r="AO150" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP150" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ150" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AU150" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV150" s="10" t="s">
         <v>201</v>
@@ -24302,7 +24308,7 @@
         <v>209</v>
       </c>
       <c r="AX150" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="151" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -24367,7 +24373,7 @@
         <v>59</v>
       </c>
       <c r="V151" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W151" s="21" t="s">
         <v>53</v>
@@ -24400,22 +24406,22 @@
         <v>147</v>
       </c>
       <c r="AL151" s="21" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AM151" s="21" t="s">
         <v>234</v>
       </c>
       <c r="AO151" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AP151" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AQ151" s="21" t="s">
         <v>152</v>
       </c>
       <c r="AU151" s="21" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AV151" s="21" t="s">
         <v>201</v>
@@ -24424,7 +24430,7 @@
         <v>209</v>
       </c>
       <c r="AX151" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -26968,12 +26974,12 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>